<commit_message>
extended to include electrical machines and drives database
</commit_message>
<xml_diff>
--- a/uc_tc.xlsx
+++ b/uc_tc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mario\trabajos2\innovación_docente_2024\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mario\trabajos2\innovación_docente_2024\ankipy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AF2499-0F19-48F8-AA3F-715187872696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCAB1A6-5D03-476A-8066-F34DF7DDB6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1813,7 +1813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DABDE3A-BB7B-4DC3-A6DB-DB47AB221C7D}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:O1"/>
     </sheetView>
   </sheetViews>
@@ -1969,7 +1969,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Actualización del fichero uc_tc.xlsx con tarjetas sobre acomplamientos magnéticos.
</commit_message>
<xml_diff>
--- a/uc_tc.xlsx
+++ b/uc_tc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mario\trabajos2\innovación_docente_2024\ankipy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{1F90608C-D3EF-4354-8C81-767D6EB413D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58E78FD1-325B-44D4-BADB-94E0FFD70529}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F5F72B-880F-43B7-96C8-267E5FA393F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6015" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="-14655" windowWidth="21600" windowHeight="11055" firstSheet="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LEEME" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="rns" sheetId="18" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_4" localSheetId="7" hidden="1">bobinas!$A$1:$J$9</definedName>
+    <definedName name="DatosExternos_4" localSheetId="7" hidden="1">bobinas!$A$1:$J$23</definedName>
     <definedName name="DatosExternos_4" localSheetId="2" hidden="1">ca!$A$1:$J$36</definedName>
     <definedName name="DatosExternos_4" localSheetId="6" hidden="1">cuadripolos!$A$1:$J$9</definedName>
     <definedName name="DatosExternos_4" localSheetId="8" hidden="1">filtros!$A$1:$J$61</definedName>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="431">
   <si>
     <t>IMPORTANTE</t>
   </si>
@@ -916,6 +916,135 @@
     <t>[latex]$V_{d}=V_{a}, V_{i}=0, V_{o}=0$ [/latex]</t>
   </si>
   <si>
+    <t>¿Cuál es la ley de Faraday?</t>
+  </si>
+  <si>
+    <t>[latex]$e=N\cdot\frac{d\Phi}{dt}$[/latex]. Si una bobina de N espiras ve un flujo magnético que varia con el tiempo, se induce una tensión en dicha bobina.</t>
+  </si>
+  <si>
+    <t>#bobinas</t>
+  </si>
+  <si>
+    <t>2. Acoplamiento Magnético</t>
+  </si>
+  <si>
+    <t>¿Cuál es la ley de Lenz?</t>
+  </si>
+  <si>
+    <t>[latex]$e=-N\cdot\frac{d\Phi}{dt}$[/latex]. La tensión inducida se opone a la corriente que produce dicho flujo magnético.</t>
+  </si>
+  <si>
+    <t>¿Cuál es la relación tensión-corriente en una bobina?</t>
+  </si>
+  <si>
+    <t>[latex]$u_{L}=L\cdot\frac{di_{L}}{dt}$[/latex]</t>
+  </si>
+  <si>
+    <t>¿Cuál es la fórmula del coeficiente de autoinducción L en una bobina en un medio lineal?</t>
+  </si>
+  <si>
+    <t>[latex]$L=N\cdot\frac{\Phi}{i}$[/latex]. Una corriente genera un flujo magnético que crece según aumenta la corriente. En un medio lineal crece indefinidamente aunque en un material real llega un punto que por mucho que aumente la corriente, no aumenta el flujo magnético.</t>
+  </si>
+  <si>
+    <t>&lt;img src="aag_flujo_corriente.png"&gt;</t>
+  </si>
+  <si>
+    <t>¿Qué representa la L de una bobina en un medio lineal?</t>
+  </si>
+  <si>
+    <t>Es la pendiente de la curva flujo vs. corriente en un medio lineal. Si L es muy grande, con poca corriente se genera mucho flujo y si L es muy pequeña, con con mucha corriente se genera poco flujo.</t>
+  </si>
+  <si>
+    <t>¿Qué es M y qué unidades tiene?</t>
+  </si>
+  <si>
+    <t>Es el coeficiente de inducción mutua y sus unidades son Henrios (H).</t>
+  </si>
+  <si>
+    <t>¿Qué es K y cómo oscila su valor entre 0 y 1?</t>
+  </si>
+  <si>
+    <t>Es el coeficiente de acoplamiento de 2 bobinas. Si las bobinas están perfectamente colocadas y todo el flujo que genera una bobina lo ve la otra (y viceversa), su valor será 1 y si están muy separadas de manera que ninguna línea de flujo de una bobina afecta a la otra (y viceversa), su valor será 0.</t>
+  </si>
+  <si>
+    <t>¿Cuáles son los pasos de la regla de los puntos para identificar la polaridad de bobinas acopladas?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Se elige un sentido para la intensidad en una de las bobinas, colocando un punto por donde entra dicha corriente. 2. Se detecta el sentido del flujo que origina dicha corriente (regla de la mano derecha). 3. Empleando la misma regla, se determina el sentido de la corriente de la segunda bobina que origina un flujo opuesto al de la primera, colocando un punto (•) por donde sale la corriente. </t>
+  </si>
+  <si>
+    <t>¿Cuál es el criterio de signos de los términos de la M y L según la regla de los puntos?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. Si las dos corrientes de las bobinas acopladas entran o salen por terminales correspondientes (con punto) los signos de los términos en M y L coinciden. B. Si una corriente de una bobina entra por el terminal con punto y la de la otra sale por su terminal correspondiente, los signos de los términos en M son opuestos a los de los términos en L. </t>
+  </si>
+  <si>
+    <t>¿Cuál es la relación entre los coeficientes de acoplamiento K y de inducción muta M?</t>
+  </si>
+  <si>
+    <t>[latex]$M=K\sqrt{L_{1}L_{2}}$[/latex]</t>
+  </si>
+  <si>
+    <t>¿Cuál es la fórmula que permite calcular la energía almacenada es dos bobinas acopladas?</t>
+  </si>
+  <si>
+    <t>[latex]$W=\frac{1}{2}L_{1}i_{1}^2+\frac{1}{2}L_{2}i_{2}^2\pm Mi_{1}i_{2}$[/latex]</t>
+  </si>
+  <si>
+    <t>¿Qué es un transformador perfecto?</t>
+  </si>
+  <si>
+    <t>Aquel transformador cuyo coeficiente de acoplamiento K e igual a 1.</t>
+  </si>
+  <si>
+    <t>¿Cuál  es el circuito eléctrico equivalente de un transformador perfecto?</t>
+  </si>
+  <si>
+    <t>&lt;img src="aag_transformador_perfecto.png"&gt;</t>
+  </si>
+  <si>
+    <t>¿Qué es un transformador ideal?</t>
+  </si>
+  <si>
+    <t>Aquel transformador que: 1) las bobinas tienen reactancias muy grandes  (L1, L2 y M tienden a infinito), 2) el coeficiente de acoplamiento es igual a la unidad (K = 1) y 3) las bobinas primaria y secundaria no tienen pérdidas (R1=R2=0).</t>
+  </si>
+  <si>
+    <t>¿Cuál  es el circuito eléctrico equivalente de un transformador ideal?</t>
+  </si>
+  <si>
+    <t>&lt;img src="aag_transformador_ideal.png"&gt;</t>
+  </si>
+  <si>
+    <t>¿Un transformador con relación 1:n es un transformador elevador o reductor?</t>
+  </si>
+  <si>
+    <t>Elevador. Por cada espira en el primario hay n espiras en el secundario.</t>
+  </si>
+  <si>
+    <t>¿Un transformador con relación n:1 es un transformador elevador o reductor?</t>
+  </si>
+  <si>
+    <t>Reductor. Por cada N espiras en el primario hay 1 espira en el secundario.</t>
+  </si>
+  <si>
+    <t>En un trasnformador ideal ¿cuál es la relación tensión, corriente, espiras e impedancia entre el primario y el secundario?</t>
+  </si>
+  <si>
+    <t>[latex]$\frac{V_{1}}{V_{2}}=\frac{N_{1}}{N_{2}}=\frac{-I_{2}}{I_{1}}=\frac{1}{n}=\sqrt{\frac{Z_{i}}{Z_{2}}}$[/latex]. Donde Zi es la impedancia de entrada o también denominada la impedancia del secundario reducida al primario.</t>
+  </si>
+  <si>
+    <t>¿Cuál es la relación entre la pontecia aparente del primario y la del secundario  en un transformador ideal?</t>
+  </si>
+  <si>
+    <t>[latex]$S_{1}=S_{2}$[/latex]</t>
+  </si>
+  <si>
+    <t>¿Qué es un autotransformador?</t>
+  </si>
+  <si>
+    <t>Es un transformador en donde el primario y el secundario se encuentran en el mismo devanado</t>
+  </si>
+  <si>
     <t>¿Qué aspecto tiene un filtro paso bajo basado en un condensador?</t>
   </si>
   <si>
@@ -1235,13 +1364,43 @@
   </si>
   <si>
     <t>[latex]$90-\arctan\frac{X_l}{R}=\arctan\frac{R}{X_l}$[/latex]</t>
+  </si>
+  <si>
+    <t>EXPORTACIÓN A IOS</t>
+  </si>
+  <si>
+    <t>.apkg</t>
+  </si>
+  <si>
+    <t>seleccionar:</t>
+  </si>
+  <si>
+    <t>Include schedluling information</t>
+  </si>
+  <si>
+    <t>Include deck presets</t>
+  </si>
+  <si>
+    <t>Include media</t>
+  </si>
+  <si>
+    <t>Support older Anki versions</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NOTA: Al exportar un mazo de cartas que tiene submazos parece que la importanción en IOS genera problemas. Aparentemente, con las opciones indicadas, y exportanto de submazo en submazo, parece que no existen problemas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1294,6 +1453,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1368,10 +1533,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1982,7 +2147,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{56121101-005F-4CFC-B5E6-47ED710B9219}" name="eadmin22248101214" displayName="eadmin22248101214" ref="A1:J9" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{56121101-005F-4CFC-B5E6-47ED710B9219}" name="eadmin22248101214" displayName="eadmin22248101214" ref="A1:J23" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{664D4462-E4BC-4AEB-89A9-7E7DC6FB0C2B}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{EA2B3F81-5C03-49DE-A5DC-719E374110C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="30"/>
@@ -2000,7 +2165,7 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{5112F37E-9CA3-427A-8B43-531951A3FB5B}" name="Tabla5379111315" displayName="Tabla5379111315" ref="K1:Y9" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{5112F37E-9CA3-427A-8B43-531951A3FB5B}" name="Tabla5379111315" displayName="Tabla5379111315" ref="K1:Y21" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{49DC50DD-FD02-438B-AB2C-7C4F0DEDAEA5}" name="Column11"/>
     <tableColumn id="2" xr3:uid="{DEB3D121-4CB7-4750-A13C-E234F05F99C2}" name="Column12"/>
@@ -2587,18 +2752,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B604BF89-0139-48FF-9E20-9314599850F7}">
-  <dimension ref="A4:H27"/>
+  <dimension ref="A4:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2606,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>2</v>
       </c>
@@ -2614,22 +2779,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -2637,7 +2802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2645,7 +2810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -2653,7 +2818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2661,7 +2826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2669,7 +2834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2677,7 +2842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2685,7 +2850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2693,7 +2858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2701,7 +2866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2709,7 +2874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2717,7 +2882,101 @@
         <v>28</v>
       </c>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>421</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>422</v>
+      </c>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>423</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>424</v>
+      </c>
+      <c r="C35" t="s">
+        <v>428</v>
+      </c>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>425</v>
+      </c>
+      <c r="C36" t="s">
+        <v>428</v>
+      </c>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>426</v>
+      </c>
+      <c r="C37" t="s">
+        <v>429</v>
+      </c>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>427</v>
+      </c>
+      <c r="C38" t="s">
+        <v>429</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E31:I38"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2731,26 +2990,26 @@
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.265625" customWidth="1"/>
+    <col min="3" max="3" width="80.59765625" customWidth="1"/>
+    <col min="4" max="4" width="80.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -2841,29 +3100,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DABDE3A-BB7B-4DC3-A6DB-DB47AB221C7D}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="D25" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="129" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="77.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.59765625" customWidth="1"/>
+    <col min="4" max="4" width="77.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.265625" customWidth="1"/>
+    <col min="6" max="6" width="8.86328125" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.25">
+    <row r="1" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -2940,7 +3199,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="14.25">
+    <row r="2" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2961,7 +3220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="14.25">
+    <row r="3" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2982,7 +3241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3003,7 +3262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3024,7 +3283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3047,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3068,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3091,7 +3350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3112,7 +3371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3135,7 +3394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3158,7 +3417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3181,7 +3440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15" customHeight="1">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3203,7 +3462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15" customHeight="1">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3225,7 +3484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15" customHeight="1">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3247,7 +3506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3269,7 +3528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3291,7 +3550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3313,7 +3572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3335,7 +3594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3357,7 +3616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3379,7 +3638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3401,7 +3660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3423,7 +3682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1">
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3445,7 +3704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3467,7 +3726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3489,7 +3748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3511,7 +3770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3532,7 +3791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1">
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3567,30 +3826,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03862EA6-EC88-47BF-BD7F-204CCEEAD41D}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.265625" customWidth="1"/>
+    <col min="3" max="3" width="80.59765625" customWidth="1"/>
+    <col min="4" max="4" width="80.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -3667,7 +3926,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3690,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="28.5">
+    <row r="3" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3713,7 +3972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="28.5">
+    <row r="4" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3736,7 +3995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="28.5">
+    <row r="5" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3759,7 +4018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="28.5">
+    <row r="6" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3782,7 +4041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="28.5">
+    <row r="7" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3805,7 +4064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="28.5">
+    <row r="8" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3828,7 +4087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="28.5">
+    <row r="9" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3851,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="28.5">
+    <row r="10" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3874,7 +4133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3897,7 +4156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="28.5">
+    <row r="12" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3920,7 +4179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="30.75">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3943,7 +4202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3966,7 +4225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3989,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4012,7 +4271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4035,7 +4294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4058,7 +4317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4081,7 +4340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4104,7 +4363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4127,7 +4386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4150,7 +4409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4173,7 +4432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4196,7 +4455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4219,7 +4478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>24</v>
       </c>
@@ -4242,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4265,7 +4524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4288,7 +4547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4311,7 +4570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="28.5">
+    <row r="30" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4334,7 +4593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="28.5">
+    <row r="31" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4357,7 +4616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="42.75">
+    <row r="32" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4384,7 +4643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4411,7 +4670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4438,7 +4697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4465,7 +4724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4510,26 +4769,26 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.265625" customWidth="1"/>
+    <col min="3" max="3" width="80.59765625" customWidth="1"/>
+    <col min="4" max="4" width="80.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.25">
+    <row r="1" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -4606,7 +4865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15" customHeight="1">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4626,7 +4885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4646,7 +4905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4666,7 +4925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4686,7 +4945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4709,7 +4968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4729,7 +4988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4752,7 +5011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="1"/>
       <c r="P9" s="1"/>
     </row>
@@ -4770,31 +5029,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F22505-FEC1-469B-890E-225C40A718B4}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:Y2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" customWidth="1"/>
+    <col min="23" max="23" width="14.59765625" customWidth="1"/>
     <col min="24" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
@@ -4871,7 +5130,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -4900,7 +5159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -4929,7 +5188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="29.25">
+    <row r="4" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -4959,7 +5218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="29.25">
+    <row r="5" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -4988,7 +5247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="29.25">
+    <row r="6" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -5015,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="29.25">
+    <row r="7" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="17">
         <v>6</v>
       </c>
@@ -5042,7 +5301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="29.25">
+    <row r="8" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -5069,7 +5328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="29.25">
+    <row r="9" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -5099,7 +5358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="29.25">
+    <row r="10" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="17">
         <v>9</v>
       </c>
@@ -5129,7 +5388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="29.25">
+    <row r="11" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="17">
         <v>10</v>
       </c>
@@ -5153,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="43.5">
+    <row r="12" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="17">
         <v>11</v>
       </c>
@@ -5180,7 +5439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="29.25">
+    <row r="13" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="17">
         <v>12</v>
       </c>
@@ -5206,7 +5465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="57.75">
+    <row r="14" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="17">
         <v>13</v>
       </c>
@@ -5230,7 +5489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="30.75">
+    <row r="15" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="17">
         <v>14</v>
       </c>
@@ -5253,7 +5512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="45.75">
+    <row r="16" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="17">
         <v>15</v>
       </c>
@@ -5280,7 +5539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="30.75">
+    <row r="17" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="17">
         <v>16</v>
       </c>
@@ -5307,7 +5566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="30.75">
+    <row r="18" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="17">
         <v>17</v>
       </c>
@@ -5334,7 +5593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="30.75">
+    <row r="19" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="17">
         <v>18</v>
       </c>
@@ -5361,7 +5620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="30.75">
+    <row r="20" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="17">
         <v>19</v>
       </c>
@@ -5388,7 +5647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="30.75">
+    <row r="21" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="17">
         <v>20</v>
       </c>
@@ -5415,7 +5674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="30.75">
+    <row r="22" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="17">
         <v>21</v>
       </c>
@@ -5442,7 +5701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="30.75">
+    <row r="23" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="17">
         <v>22</v>
       </c>
@@ -5465,7 +5724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="30.75">
+    <row r="24" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="17">
         <v>23</v>
       </c>
@@ -5488,7 +5747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="29.25">
+    <row r="25" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="17">
         <v>24</v>
       </c>
@@ -5511,7 +5770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="57.75">
+    <row r="26" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="17">
         <v>25</v>
       </c>
@@ -5534,7 +5793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="57.75">
+    <row r="27" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="17">
         <v>26</v>
       </c>
@@ -5557,7 +5816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="57.75">
+    <row r="28" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A28" s="17">
         <v>27</v>
       </c>
@@ -5580,7 +5839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="57.75">
+    <row r="29" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="17">
         <v>28</v>
       </c>
@@ -5603,7 +5862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="87">
+    <row r="30" spans="1:25" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A30" s="17">
         <v>29</v>
       </c>
@@ -5629,7 +5888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="72.75">
+    <row r="31" spans="1:25" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A31" s="17">
         <v>30</v>
       </c>
@@ -5655,7 +5914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="43.5">
+    <row r="32" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="17">
         <v>31</v>
       </c>
@@ -5675,7 +5934,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="43.5">
+    <row r="33" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="17">
         <v>32</v>
       </c>
@@ -5695,7 +5954,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="29.25">
+    <row r="34" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="17">
         <v>33</v>
       </c>
@@ -5715,23 +5974,16 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="29.25">
+    <row r="35" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="17">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C35" s="19"/>
       <c r="D35" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
       <c r="P35" t="s">
         <v>196</v>
       </c>
@@ -5742,23 +5994,16 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="29.25">
+    <row r="36" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A36" s="17">
         <v>35</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
       <c r="P36" t="s">
         <v>196</v>
       </c>
@@ -5787,26 +6032,26 @@
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.265625" customWidth="1"/>
+    <col min="3" max="3" width="80.59765625" customWidth="1"/>
+    <col min="4" max="4" width="80.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -5901,26 +6146,26 @@
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.265625" customWidth="1"/>
+    <col min="3" max="3" width="80.59765625" customWidth="1"/>
+    <col min="4" max="4" width="80.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -6009,32 +6254,33 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16062F6-9546-4DC3-BF7B-DAC218FC8CC2}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.265625" customWidth="1"/>
+    <col min="3" max="3" width="34.73046875" customWidth="1"/>
+    <col min="4" max="4" width="89.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
-    <col min="23" max="25" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -6109,6 +6355,410 @@
       </c>
       <c r="Y1" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="P2" t="s">
+        <v>273</v>
+      </c>
+      <c r="R2" t="s">
+        <v>197</v>
+      </c>
+      <c r="W2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="P3" t="s">
+        <v>273</v>
+      </c>
+      <c r="R3" t="s">
+        <v>197</v>
+      </c>
+      <c r="W3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="P4" t="s">
+        <v>273</v>
+      </c>
+      <c r="R4" t="s">
+        <v>197</v>
+      </c>
+      <c r="W4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E5" t="s">
+        <v>281</v>
+      </c>
+      <c r="P5" t="s">
+        <v>273</v>
+      </c>
+      <c r="R5" t="s">
+        <v>197</v>
+      </c>
+      <c r="W5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="P6" t="s">
+        <v>273</v>
+      </c>
+      <c r="R6" t="s">
+        <v>197</v>
+      </c>
+      <c r="W6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="P7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R7" t="s">
+        <v>197</v>
+      </c>
+      <c r="W7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="P8" t="s">
+        <v>273</v>
+      </c>
+      <c r="R8" t="s">
+        <v>197</v>
+      </c>
+      <c r="W8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="57" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="P9" t="s">
+        <v>273</v>
+      </c>
+      <c r="R9" t="s">
+        <v>197</v>
+      </c>
+      <c r="W9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="57" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="P10" t="s">
+        <v>273</v>
+      </c>
+      <c r="R10" t="s">
+        <v>197</v>
+      </c>
+      <c r="W10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="P11" t="s">
+        <v>273</v>
+      </c>
+      <c r="R11" t="s">
+        <v>197</v>
+      </c>
+      <c r="W11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="P12" t="s">
+        <v>273</v>
+      </c>
+      <c r="R12" t="s">
+        <v>197</v>
+      </c>
+      <c r="W12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="P13" t="s">
+        <v>273</v>
+      </c>
+      <c r="R13" t="s">
+        <v>197</v>
+      </c>
+      <c r="W13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>298</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="P14" t="s">
+        <v>273</v>
+      </c>
+      <c r="R14" t="s">
+        <v>197</v>
+      </c>
+      <c r="W14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>300</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="P15" t="s">
+        <v>273</v>
+      </c>
+      <c r="R15" t="s">
+        <v>197</v>
+      </c>
+      <c r="W15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>302</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="P16" t="s">
+        <v>273</v>
+      </c>
+      <c r="R16" t="s">
+        <v>197</v>
+      </c>
+      <c r="W16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="P17" t="s">
+        <v>273</v>
+      </c>
+      <c r="R17" t="s">
+        <v>197</v>
+      </c>
+      <c r="W17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="P18" t="s">
+        <v>273</v>
+      </c>
+      <c r="R18" t="s">
+        <v>197</v>
+      </c>
+      <c r="W18" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="P19" t="s">
+        <v>273</v>
+      </c>
+      <c r="R19" t="s">
+        <v>197</v>
+      </c>
+      <c r="W19" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="P20" t="s">
+        <v>273</v>
+      </c>
+      <c r="R20" t="s">
+        <v>197</v>
+      </c>
+      <c r="W20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="P21" t="s">
+        <v>273</v>
+      </c>
+      <c r="R21" t="s">
+        <v>197</v>
+      </c>
+      <c r="W21" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -6129,28 +6779,28 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.59765625" customWidth="1"/>
+    <col min="4" max="4" width="80.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="10.86328125" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.59765625" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
-    <col min="23" max="23" width="22.42578125" customWidth="1"/>
-    <col min="24" max="24" width="18.28515625" customWidth="1"/>
+    <col min="23" max="23" width="22.3984375" customWidth="1"/>
+    <col min="24" max="24" width="18.265625" customWidth="1"/>
     <col min="25" max="26" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -6227,17 +6877,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1">
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>271</v>
+        <v>314</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="6"/>
       <c r="E2" s="14" t="s">
-        <v>272</v>
+        <v>315</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -6250,18 +6900,18 @@
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
       <c r="P2" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q2" s="13"/>
       <c r="R2" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
       <c r="V2" s="13"/>
       <c r="W2" s="13" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X2" s="13"/>
       <c r="Y2" s="13"/>
@@ -6269,17 +6919,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1">
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>276</v>
+        <v>319</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="6"/>
       <c r="E3" s="14" t="s">
-        <v>277</v>
+        <v>320</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -6292,18 +6942,18 @@
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q3" s="13"/>
       <c r="R3" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
       <c r="W3" s="13" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X3" s="13"/>
       <c r="Y3" s="13"/>
@@ -6311,17 +6961,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="13">
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>278</v>
+        <v>321</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="6"/>
       <c r="E4" s="14" t="s">
-        <v>279</v>
+        <v>322</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -6334,18 +6984,18 @@
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q4" s="13"/>
       <c r="R4" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
       <c r="U4" s="13"/>
       <c r="V4" s="13"/>
       <c r="W4" s="13" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
@@ -6353,17 +7003,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>280</v>
+        <v>323</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="6"/>
       <c r="E5" s="14" t="s">
-        <v>281</v>
+        <v>324</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -6376,18 +7026,18 @@
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q5" s="13"/>
       <c r="R5" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S5" s="13"/>
       <c r="T5" s="13"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
       <c r="W5" s="13" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
@@ -6395,17 +7045,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>282</v>
+        <v>325</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="6"/>
       <c r="E6" s="14" t="s">
-        <v>283</v>
+        <v>326</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -6418,18 +7068,18 @@
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q6" s="13"/>
       <c r="R6" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
       <c r="U6" s="13"/>
       <c r="V6" s="13"/>
       <c r="W6" s="13" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
@@ -6437,17 +7087,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1">
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>284</v>
+        <v>327</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="6"/>
       <c r="E7" s="14" t="s">
-        <v>285</v>
+        <v>328</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -6460,18 +7110,18 @@
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q7" s="13"/>
       <c r="R7" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S7" s="13"/>
       <c r="T7" s="13"/>
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
       <c r="W7" s="13" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
@@ -6479,17 +7129,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1">
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>286</v>
+        <v>329</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="6"/>
       <c r="E8" s="14" t="s">
-        <v>287</v>
+        <v>330</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -6502,18 +7152,18 @@
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q8" s="13"/>
       <c r="R8" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
       <c r="W8" s="13" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X8" s="13"/>
       <c r="Y8" s="13"/>
@@ -6521,17 +7171,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1">
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>288</v>
+        <v>331</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="6"/>
       <c r="E9" s="14" t="s">
-        <v>289</v>
+        <v>332</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -6544,18 +7194,18 @@
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q9" s="13"/>
       <c r="R9" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S9" s="13"/>
       <c r="T9" s="13"/>
       <c r="U9" s="13"/>
       <c r="V9" s="13"/>
       <c r="W9" s="13" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
@@ -6563,17 +7213,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1">
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="13">
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>290</v>
+        <v>333</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="6"/>
       <c r="E10" s="14" t="s">
-        <v>291</v>
+        <v>334</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -6586,18 +7236,18 @@
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q10" s="13"/>
       <c r="R10" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
       <c r="W10" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
@@ -6605,17 +7255,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1">
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>292</v>
+        <v>335</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="6"/>
       <c r="E11" s="14" t="s">
-        <v>293</v>
+        <v>336</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -6628,18 +7278,18 @@
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q11" s="13"/>
       <c r="R11" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
       <c r="U11" s="13"/>
       <c r="V11" s="13"/>
       <c r="W11" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -6647,16 +7297,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1">
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="13">
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>294</v>
+        <v>337</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="6" t="s">
-        <v>295</v>
+        <v>338</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="13"/>
@@ -6670,18 +7320,18 @@
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q12" s="13"/>
       <c r="R12" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
       <c r="W12" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
@@ -6689,16 +7339,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1">
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="13">
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>296</v>
+        <v>339</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="6" t="s">
-        <v>297</v>
+        <v>340</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -6712,18 +7362,18 @@
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q13" s="13"/>
       <c r="R13" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
       <c r="W13" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -6731,16 +7381,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1">
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>298</v>
+        <v>341</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="6" t="s">
-        <v>295</v>
+        <v>338</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -6754,18 +7404,18 @@
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
       <c r="P14" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q14" s="13"/>
       <c r="R14" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
       <c r="W14" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
@@ -6773,16 +7423,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1">
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>299</v>
+        <v>342</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="6" t="s">
-        <v>295</v>
+        <v>338</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -6796,18 +7446,18 @@
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q15" s="13"/>
       <c r="R15" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
       <c r="V15" s="13"/>
       <c r="W15" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -6815,16 +7465,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1">
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="13">
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>300</v>
+        <v>343</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="6" t="s">
-        <v>295</v>
+        <v>338</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -6838,18 +7488,18 @@
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
       <c r="P16" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S16" s="13"/>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
       <c r="W16" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -6857,16 +7507,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="15" customHeight="1">
+    <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="13">
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>301</v>
+        <v>344</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="6" t="s">
-        <v>297</v>
+        <v>340</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -6880,18 +7530,18 @@
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q17" s="13"/>
       <c r="R17" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S17" s="13"/>
       <c r="T17" s="13"/>
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
       <c r="W17" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -6899,16 +7549,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="15" customHeight="1">
+    <row r="18" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="13">
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>302</v>
+        <v>345</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="6" t="s">
-        <v>303</v>
+        <v>346</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -6922,18 +7572,18 @@
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q18" s="13"/>
       <c r="R18" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S18" s="13"/>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
       <c r="V18" s="13"/>
       <c r="W18" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
@@ -6941,16 +7591,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="15" customHeight="1">
+    <row r="19" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="13">
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>304</v>
+        <v>347</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="6" t="s">
-        <v>295</v>
+        <v>338</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
@@ -6964,18 +7614,18 @@
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q19" s="13"/>
       <c r="R19" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
       <c r="V19" s="13"/>
       <c r="W19" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -6983,16 +7633,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="15" customHeight="1">
+    <row r="20" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="13">
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>305</v>
+        <v>348</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="6" t="s">
-        <v>295</v>
+        <v>338</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
@@ -7006,18 +7656,18 @@
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
       <c r="P20" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q20" s="13"/>
       <c r="R20" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S20" s="13"/>
       <c r="T20" s="13"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
       <c r="W20" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X20" s="13"/>
       <c r="Y20" s="13"/>
@@ -7025,16 +7675,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="15" customHeight="1">
+    <row r="21" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="13">
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>306</v>
+        <v>349</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="6" t="s">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -7048,18 +7698,18 @@
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q21" s="13"/>
       <c r="R21" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S21" s="13"/>
       <c r="T21" s="13"/>
       <c r="U21" s="13"/>
       <c r="V21" s="13"/>
       <c r="W21" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X21" s="13"/>
       <c r="Y21" s="13"/>
@@ -7067,16 +7717,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="15" customHeight="1">
+    <row r="22" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="13">
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>308</v>
+        <v>351</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="6" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -7090,18 +7740,18 @@
       <c r="N22" s="13"/>
       <c r="O22" s="13"/>
       <c r="P22" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q22" s="13"/>
       <c r="R22" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S22" s="13"/>
       <c r="T22" s="13"/>
       <c r="U22" s="13"/>
       <c r="V22" s="13"/>
       <c r="W22" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
@@ -7109,16 +7759,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="15" customHeight="1">
+    <row r="23" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="13">
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="6" t="s">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
@@ -7132,18 +7782,18 @@
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
       <c r="P23" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q23" s="13"/>
       <c r="R23" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S23" s="13"/>
       <c r="T23" s="13"/>
       <c r="U23" s="13"/>
       <c r="V23" s="13"/>
       <c r="W23" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -7151,16 +7801,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="15" customHeight="1">
+    <row r="24" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="13">
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>311</v>
+        <v>354</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="6" t="s">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
@@ -7174,18 +7824,18 @@
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
       <c r="P24" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q24" s="13"/>
       <c r="R24" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S24" s="13"/>
       <c r="T24" s="13"/>
       <c r="U24" s="13"/>
       <c r="V24" s="13"/>
       <c r="W24" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -7193,16 +7843,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15" customHeight="1">
+    <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="13">
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>312</v>
+        <v>355</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="6" t="s">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
@@ -7216,18 +7866,18 @@
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
       <c r="P25" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q25" s="13"/>
       <c r="R25" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S25" s="13"/>
       <c r="T25" s="13"/>
       <c r="U25" s="13"/>
       <c r="V25" s="13"/>
       <c r="W25" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
@@ -7235,16 +7885,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="15" customHeight="1">
+    <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="13">
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>313</v>
+        <v>356</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="6" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
@@ -7258,18 +7908,18 @@
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
       <c r="P26" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q26" s="13"/>
       <c r="R26" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S26" s="13"/>
       <c r="T26" s="13"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
       <c r="W26" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X26" s="13"/>
       <c r="Y26" s="13"/>
@@ -7277,16 +7927,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="15" customHeight="1">
+    <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="13">
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>314</v>
+        <v>357</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="6" t="s">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
@@ -7300,18 +7950,18 @@
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q27" s="13"/>
       <c r="R27" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S27" s="13"/>
       <c r="T27" s="13"/>
       <c r="U27" s="13"/>
       <c r="V27" s="13"/>
       <c r="W27" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X27" s="13"/>
       <c r="Y27" s="13"/>
@@ -7319,16 +7969,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="15" customHeight="1">
+    <row r="28" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="13">
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>315</v>
+        <v>358</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="6" t="s">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
@@ -7342,18 +7992,18 @@
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q28" s="13"/>
       <c r="R28" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S28" s="13"/>
       <c r="T28" s="13"/>
       <c r="U28" s="13"/>
       <c r="V28" s="13"/>
       <c r="W28" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -7361,16 +8011,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="15" customHeight="1">
+    <row r="29" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="13">
         <v>28</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>316</v>
+        <v>359</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="6" t="s">
-        <v>317</v>
+        <v>360</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
@@ -7384,18 +8034,18 @@
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
       <c r="P29" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q29" s="13"/>
       <c r="R29" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S29" s="13"/>
       <c r="T29" s="13"/>
       <c r="U29" s="13"/>
       <c r="V29" s="13"/>
       <c r="W29" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
@@ -7403,16 +8053,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="15" customHeight="1">
+    <row r="30" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="13">
         <v>29</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>318</v>
+        <v>361</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="6" t="s">
-        <v>319</v>
+        <v>362</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
@@ -7426,18 +8076,18 @@
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
       <c r="P30" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q30" s="13"/>
       <c r="R30" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="13"/>
       <c r="V30" s="13"/>
       <c r="W30" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X30" s="13"/>
       <c r="Y30" s="13"/>
@@ -7445,16 +8095,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="15" customHeight="1">
+    <row r="31" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="13">
         <v>30</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>320</v>
+        <v>363</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="6" t="s">
-        <v>317</v>
+        <v>360</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
@@ -7468,18 +8118,18 @@
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
       <c r="P31" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q31" s="13"/>
       <c r="R31" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S31" s="13"/>
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
       <c r="W31" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
@@ -7487,16 +8137,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="15" customHeight="1">
+    <row r="32" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="13">
         <v>31</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>321</v>
+        <v>364</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="6" t="s">
-        <v>319</v>
+        <v>362</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
@@ -7510,18 +8160,18 @@
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
       <c r="P32" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q32" s="13"/>
       <c r="R32" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S32" s="13"/>
       <c r="T32" s="13"/>
       <c r="U32" s="13"/>
       <c r="V32" s="13"/>
       <c r="W32" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
@@ -7529,16 +8179,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="15" customHeight="1">
+    <row r="33" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="13">
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>322</v>
+        <v>365</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="6" t="s">
-        <v>323</v>
+        <v>366</v>
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
@@ -7552,18 +8202,18 @@
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
       <c r="P33" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q33" s="13"/>
       <c r="R33" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S33" s="13"/>
       <c r="T33" s="13"/>
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
       <c r="W33" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
@@ -7571,16 +8221,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="15" customHeight="1">
+    <row r="34" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="13">
         <v>33</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>324</v>
+        <v>367</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="6" t="s">
-        <v>325</v>
+        <v>368</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
@@ -7594,18 +8244,18 @@
       <c r="N34" s="13"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q34" s="13"/>
       <c r="R34" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S34" s="13"/>
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
       <c r="V34" s="13"/>
       <c r="W34" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X34" s="13"/>
       <c r="Y34" s="13"/>
@@ -7613,16 +8263,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="15" customHeight="1">
+    <row r="35" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="13">
         <v>34</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>326</v>
+        <v>369</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="6" t="s">
-        <v>323</v>
+        <v>366</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
@@ -7636,18 +8286,18 @@
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q35" s="13"/>
       <c r="R35" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
       <c r="V35" s="13"/>
       <c r="W35" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X35" s="13"/>
       <c r="Y35" s="13"/>
@@ -7655,16 +8305,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="15" customHeight="1">
+    <row r="36" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="13">
         <v>35</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>327</v>
+        <v>370</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="6" t="s">
-        <v>325</v>
+        <v>368</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
@@ -7678,18 +8328,18 @@
       <c r="N36" s="13"/>
       <c r="O36" s="13"/>
       <c r="P36" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q36" s="13"/>
       <c r="R36" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S36" s="13"/>
       <c r="T36" s="13"/>
       <c r="U36" s="13"/>
       <c r="V36" s="13"/>
       <c r="W36" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
@@ -7697,16 +8347,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="15" customHeight="1">
+    <row r="37" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="13">
         <v>36</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>328</v>
+        <v>371</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="6" t="s">
-        <v>329</v>
+        <v>372</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
@@ -7720,18 +8370,18 @@
       <c r="N37" s="13"/>
       <c r="O37" s="13"/>
       <c r="P37" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q37" s="13"/>
       <c r="R37" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S37" s="13"/>
       <c r="T37" s="13"/>
       <c r="U37" s="13"/>
       <c r="V37" s="13"/>
       <c r="W37" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X37" s="13"/>
       <c r="Y37" s="13"/>
@@ -7739,16 +8389,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="15" customHeight="1">
+    <row r="38" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="13">
         <v>37</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>330</v>
+        <v>373</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="6" t="s">
-        <v>331</v>
+        <v>374</v>
       </c>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
@@ -7762,18 +8412,18 @@
       <c r="N38" s="13"/>
       <c r="O38" s="13"/>
       <c r="P38" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q38" s="13"/>
       <c r="R38" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S38" s="13"/>
       <c r="T38" s="13"/>
       <c r="U38" s="13"/>
       <c r="V38" s="13"/>
       <c r="W38" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X38" s="13"/>
       <c r="Y38" s="13"/>
@@ -7781,16 +8431,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="15" customHeight="1">
+    <row r="39" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="13">
         <v>38</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>332</v>
+        <v>375</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="6" t="s">
-        <v>333</v>
+        <v>376</v>
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
@@ -7804,18 +8454,18 @@
       <c r="N39" s="13"/>
       <c r="O39" s="13"/>
       <c r="P39" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q39" s="13"/>
       <c r="R39" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S39" s="13"/>
       <c r="T39" s="13"/>
       <c r="U39" s="13"/>
       <c r="V39" s="13"/>
       <c r="W39" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X39" s="13"/>
       <c r="Y39" s="13"/>
@@ -7823,16 +8473,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="15" customHeight="1">
+    <row r="40" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="13">
         <v>39</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>334</v>
+        <v>377</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="6" t="s">
-        <v>335</v>
+        <v>378</v>
       </c>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
@@ -7846,18 +8496,18 @@
       <c r="N40" s="13"/>
       <c r="O40" s="13"/>
       <c r="P40" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q40" s="13"/>
       <c r="R40" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
       <c r="U40" s="13"/>
       <c r="V40" s="13"/>
       <c r="W40" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X40" s="13"/>
       <c r="Y40" s="13"/>
@@ -7865,16 +8515,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="15" customHeight="1">
+    <row r="41" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="13">
         <v>40</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>336</v>
+        <v>379</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="6" t="s">
-        <v>337</v>
+        <v>380</v>
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
@@ -7888,18 +8538,18 @@
       <c r="N41" s="13"/>
       <c r="O41" s="13"/>
       <c r="P41" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q41" s="13"/>
       <c r="R41" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S41" s="13"/>
       <c r="T41" s="13"/>
       <c r="U41" s="13"/>
       <c r="V41" s="13"/>
       <c r="W41" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X41" s="13"/>
       <c r="Y41" s="13"/>
@@ -7907,16 +8557,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="15" customHeight="1">
+    <row r="42" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="13">
         <v>41</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>338</v>
+        <v>381</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="6" t="s">
-        <v>339</v>
+        <v>382</v>
       </c>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
@@ -7930,18 +8580,18 @@
       <c r="N42" s="13"/>
       <c r="O42" s="13"/>
       <c r="P42" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q42" s="13"/>
       <c r="R42" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S42" s="13"/>
       <c r="T42" s="13"/>
       <c r="U42" s="13"/>
       <c r="V42" s="13"/>
       <c r="W42" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X42" s="13"/>
       <c r="Y42" s="13"/>
@@ -7949,16 +8599,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="15" customHeight="1">
+    <row r="43" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="13">
         <v>42</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>340</v>
+        <v>383</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="6" t="s">
-        <v>341</v>
+        <v>384</v>
       </c>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
@@ -7972,18 +8622,18 @@
       <c r="N43" s="13"/>
       <c r="O43" s="13"/>
       <c r="P43" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q43" s="13"/>
       <c r="R43" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S43" s="13"/>
       <c r="T43" s="13"/>
       <c r="U43" s="13"/>
       <c r="V43" s="13"/>
       <c r="W43" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X43" s="13"/>
       <c r="Y43" s="13"/>
@@ -7991,16 +8641,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="15" customHeight="1">
+    <row r="44" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="13">
         <v>43</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>342</v>
+        <v>385</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="6" t="s">
-        <v>343</v>
+        <v>386</v>
       </c>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
@@ -8014,18 +8664,18 @@
       <c r="N44" s="13"/>
       <c r="O44" s="13"/>
       <c r="P44" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q44" s="13"/>
       <c r="R44" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S44" s="13"/>
       <c r="T44" s="13"/>
       <c r="U44" s="13"/>
       <c r="V44" s="13"/>
       <c r="W44" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X44" s="13"/>
       <c r="Y44" s="13"/>
@@ -8033,16 +8683,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="15" customHeight="1">
+    <row r="45" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="13">
         <v>44</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="6" t="s">
-        <v>345</v>
+        <v>388</v>
       </c>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
@@ -8056,18 +8706,18 @@
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
       <c r="P45" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q45" s="13"/>
       <c r="R45" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S45" s="13"/>
       <c r="T45" s="13"/>
       <c r="U45" s="13"/>
       <c r="V45" s="13"/>
       <c r="W45" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X45" s="13"/>
       <c r="Y45" s="13"/>
@@ -8075,16 +8725,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="15" customHeight="1">
+    <row r="46" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="13">
         <v>45</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>346</v>
+        <v>389</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="6" t="s">
-        <v>347</v>
+        <v>390</v>
       </c>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
@@ -8098,18 +8748,18 @@
       <c r="N46" s="13"/>
       <c r="O46" s="13"/>
       <c r="P46" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q46" s="13"/>
       <c r="R46" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S46" s="13"/>
       <c r="T46" s="13"/>
       <c r="U46" s="13"/>
       <c r="V46" s="13"/>
       <c r="W46" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X46" s="13"/>
       <c r="Y46" s="13"/>
@@ -8117,16 +8767,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="15" customHeight="1">
+    <row r="47" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="13">
         <v>46</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>348</v>
+        <v>391</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="6" t="s">
-        <v>349</v>
+        <v>392</v>
       </c>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
@@ -8140,18 +8790,18 @@
       <c r="N47" s="13"/>
       <c r="O47" s="13"/>
       <c r="P47" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q47" s="13"/>
       <c r="R47" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S47" s="13"/>
       <c r="T47" s="13"/>
       <c r="U47" s="13"/>
       <c r="V47" s="13"/>
       <c r="W47" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X47" s="13"/>
       <c r="Y47" s="13"/>
@@ -8159,16 +8809,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="15" customHeight="1">
+    <row r="48" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="13">
         <v>47</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="6" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
@@ -8182,18 +8832,18 @@
       <c r="N48" s="13"/>
       <c r="O48" s="13"/>
       <c r="P48" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q48" s="13"/>
       <c r="R48" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S48" s="13"/>
       <c r="T48" s="13"/>
       <c r="U48" s="13"/>
       <c r="V48" s="13"/>
       <c r="W48" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X48" s="13"/>
       <c r="Y48" s="13"/>
@@ -8201,16 +8851,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="15" customHeight="1">
+    <row r="49" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="13">
         <v>48</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>352</v>
+        <v>395</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="6" t="s">
-        <v>353</v>
+        <v>396</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -8224,18 +8874,18 @@
       <c r="N49" s="13"/>
       <c r="O49" s="13"/>
       <c r="P49" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q49" s="13"/>
       <c r="R49" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S49" s="13"/>
       <c r="T49" s="13"/>
       <c r="U49" s="13"/>
       <c r="V49" s="13"/>
       <c r="W49" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X49" s="13"/>
       <c r="Y49" s="13"/>
@@ -8243,16 +8893,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="15" customHeight="1">
+    <row r="50" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="13">
         <v>49</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>354</v>
+        <v>397</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="6" t="s">
-        <v>355</v>
+        <v>398</v>
       </c>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -8266,18 +8916,18 @@
       <c r="N50" s="13"/>
       <c r="O50" s="13"/>
       <c r="P50" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q50" s="13"/>
       <c r="R50" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S50" s="13"/>
       <c r="T50" s="13"/>
       <c r="U50" s="13"/>
       <c r="V50" s="13"/>
       <c r="W50" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X50" s="13"/>
       <c r="Y50" s="13"/>
@@ -8285,16 +8935,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="15" customHeight="1">
+    <row r="51" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="13">
         <v>50</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>356</v>
+        <v>399</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="6" t="s">
-        <v>357</v>
+        <v>400</v>
       </c>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
@@ -8308,18 +8958,18 @@
       <c r="N51" s="13"/>
       <c r="O51" s="13"/>
       <c r="P51" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q51" s="13"/>
       <c r="R51" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S51" s="13"/>
       <c r="T51" s="13"/>
       <c r="U51" s="13"/>
       <c r="V51" s="13"/>
       <c r="W51" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X51" s="13"/>
       <c r="Y51" s="13"/>
@@ -8327,16 +8977,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="15" customHeight="1">
+    <row r="52" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="13">
         <v>51</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>358</v>
+        <v>401</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="6" t="s">
-        <v>359</v>
+        <v>402</v>
       </c>
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
@@ -8350,18 +9000,18 @@
       <c r="N52" s="13"/>
       <c r="O52" s="13"/>
       <c r="P52" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q52" s="13"/>
       <c r="R52" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S52" s="13"/>
       <c r="T52" s="13"/>
       <c r="U52" s="13"/>
       <c r="V52" s="13"/>
       <c r="W52" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X52" s="13"/>
       <c r="Y52" s="13"/>
@@ -8369,16 +9019,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="15" customHeight="1">
+    <row r="53" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="13">
         <v>52</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>360</v>
+        <v>403</v>
       </c>
       <c r="C53" s="13"/>
       <c r="D53" s="6" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
@@ -8392,18 +9042,18 @@
       <c r="N53" s="13"/>
       <c r="O53" s="13"/>
       <c r="P53" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q53" s="13"/>
       <c r="R53" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S53" s="13"/>
       <c r="T53" s="13"/>
       <c r="U53" s="13"/>
       <c r="V53" s="13"/>
       <c r="W53" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X53" s="13"/>
       <c r="Y53" s="13"/>
@@ -8411,16 +9061,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="15" customHeight="1">
+    <row r="54" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="13">
         <v>53</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>362</v>
+        <v>405</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="6" t="s">
-        <v>363</v>
+        <v>406</v>
       </c>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
@@ -8434,18 +9084,18 @@
       <c r="N54" s="13"/>
       <c r="O54" s="13"/>
       <c r="P54" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q54" s="13"/>
       <c r="R54" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S54" s="13"/>
       <c r="T54" s="13"/>
       <c r="U54" s="13"/>
       <c r="V54" s="13"/>
       <c r="W54" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X54" s="13"/>
       <c r="Y54" s="13"/>
@@ -8453,16 +9103,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="15" customHeight="1">
+    <row r="55" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="13">
         <v>54</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>364</v>
+        <v>407</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="6" t="s">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
@@ -8476,18 +9126,18 @@
       <c r="N55" s="13"/>
       <c r="O55" s="13"/>
       <c r="P55" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q55" s="13"/>
       <c r="R55" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S55" s="13"/>
       <c r="T55" s="13"/>
       <c r="U55" s="13"/>
       <c r="V55" s="13"/>
       <c r="W55" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X55" s="13"/>
       <c r="Y55" s="13"/>
@@ -8495,16 +9145,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="15" customHeight="1">
+    <row r="56" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="13">
         <v>55</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>366</v>
+        <v>409</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="6" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
@@ -8518,18 +9168,18 @@
       <c r="N56" s="13"/>
       <c r="O56" s="13"/>
       <c r="P56" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q56" s="13"/>
       <c r="R56" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S56" s="13"/>
       <c r="T56" s="13"/>
       <c r="U56" s="13"/>
       <c r="V56" s="13"/>
       <c r="W56" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X56" s="13"/>
       <c r="Y56" s="13"/>
@@ -8537,16 +9187,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="15" customHeight="1">
+    <row r="57" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="13">
         <v>56</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>368</v>
+        <v>411</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="6" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
@@ -8560,18 +9210,18 @@
       <c r="N57" s="13"/>
       <c r="O57" s="13"/>
       <c r="P57" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q57" s="13"/>
       <c r="R57" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S57" s="13"/>
       <c r="T57" s="13"/>
       <c r="U57" s="13"/>
       <c r="V57" s="13"/>
       <c r="W57" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X57" s="13"/>
       <c r="Y57" s="13"/>
@@ -8579,16 +9229,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="15" customHeight="1">
+    <row r="58" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="13">
         <v>57</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>370</v>
+        <v>413</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="6" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
@@ -8602,18 +9252,18 @@
       <c r="N58" s="13"/>
       <c r="O58" s="13"/>
       <c r="P58" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q58" s="13"/>
       <c r="R58" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S58" s="13"/>
       <c r="T58" s="13"/>
       <c r="U58" s="13"/>
       <c r="V58" s="13"/>
       <c r="W58" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X58" s="13"/>
       <c r="Y58" s="13"/>
@@ -8621,16 +9271,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="15" customHeight="1">
+    <row r="59" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="13">
         <v>58</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>372</v>
+        <v>415</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="6" t="s">
-        <v>373</v>
+        <v>416</v>
       </c>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
@@ -8644,18 +9294,18 @@
       <c r="N59" s="13"/>
       <c r="O59" s="13"/>
       <c r="P59" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q59" s="13"/>
       <c r="R59" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S59" s="13"/>
       <c r="T59" s="13"/>
       <c r="U59" s="13"/>
       <c r="V59" s="13"/>
       <c r="W59" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X59" s="13"/>
       <c r="Y59" s="13"/>
@@ -8663,16 +9313,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="15" customHeight="1">
+    <row r="60" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="13">
         <v>59</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="6" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="E60" s="13"/>
       <c r="F60" s="13"/>
@@ -8686,18 +9336,18 @@
       <c r="N60" s="13"/>
       <c r="O60" s="13"/>
       <c r="P60" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q60" s="13"/>
       <c r="R60" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S60" s="13"/>
       <c r="T60" s="13"/>
       <c r="U60" s="13"/>
       <c r="V60" s="13"/>
       <c r="W60" s="16" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X60" s="13"/>
       <c r="Y60" s="13"/>
@@ -8705,16 +9355,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="15" customHeight="1">
+    <row r="61" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="13">
         <v>60</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="6" t="s">
-        <v>377</v>
+        <v>420</v>
       </c>
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
@@ -8728,18 +9378,18 @@
       <c r="N61" s="13"/>
       <c r="O61" s="13"/>
       <c r="P61" s="13" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="Q61" s="13"/>
       <c r="R61" s="13" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="S61" s="13"/>
       <c r="T61" s="13"/>
       <c r="U61" s="13"/>
       <c r="V61" s="13"/>
       <c r="W61" s="15" t="s">
-        <v>275</v>
+        <v>318</v>
       </c>
       <c r="X61" s="13"/>
       <c r="Y61" s="13"/>
@@ -8761,5 +9411,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A152E4B2-D709-4333-8EF0-22FFF9B55442}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A152E4B2-D709-4333-8EF0-22FFF9B55442}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>